<commit_message>
Add configuration files and implement BERTopic clustering functionality
</commit_message>
<xml_diff>
--- a/out_rev/priceUnit_LCOE_clean.xlsx
+++ b/out_rev/priceUnit_LCOE_clean.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
   <si>
     <t xml:space="preserve">unit</t>
   </si>
@@ -184,6 +184,9 @@
     <t xml:space="preserve">to  euro/mwh</t>
   </si>
   <si>
+    <t xml:space="preserve">v = v.replace('megawatthour', 'MWh')</t>
+  </si>
+  <si>
     <t xml:space="preserve">€</t>
   </si>
   <si>
@@ -193,6 +196,12 @@
     <t xml:space="preserve">c$/kwh</t>
   </si>
   <si>
+    <t xml:space="preserve">USDc/kWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EURc/kWh</t>
+  </si>
+  <si>
     <t xml:space="preserve">EURkwh</t>
   </si>
   <si>
@@ -209,6 +218,9 @@
   </si>
   <si>
     <t xml:space="preserve">USDkWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EURkWh</t>
   </si>
 </sst>
 </file>
@@ -304,7 +316,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,10 +334,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -521,10 +529,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -964,8 +972,8 @@
       <c r="A44" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="1" t="n">
-        <v>2</v>
+      <c r="B44" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>21</v>
@@ -973,7 +981,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>3</v>
@@ -981,7 +989,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>2</v>
@@ -992,7 +1000,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>1</v>
@@ -1043,23 +1051,18 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="C54" s="1"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>31</v>
@@ -1091,7 +1094,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>19</v>
@@ -1099,7 +1102,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>44</v>
@@ -1107,23 +1110,23 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C62" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>9</v>
@@ -1131,10 +1134,18 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>5</v>
+        <v>65</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>